<commit_message>
hedges.py fix: pooled SD for two measurments
</commit_message>
<xml_diff>
--- a/tests/multi_samples.xlsx
+++ b/tests/multi_samples.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DCPROGS\RANTEST\tests\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{503330F4-2FC0-465C-BECA-836A82E077E6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="EC50" sheetId="1" r:id="rId1"/>
+    <sheet name="two_measurments" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>a1bWTg</t>
   </si>
@@ -38,12 +33,18 @@
   </si>
   <si>
     <t>a1S270Ts</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -135,7 +136,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -168,26 +169,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -220,23 +204,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -412,14 +379,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -596,4 +563,43 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>